<commit_message>
Edited git commant file
</commit_message>
<xml_diff>
--- a/Git_command.xlsx
+++ b/Git_command.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_repos\Online_retail_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E3A7A4-8A8B-45F6-A37A-1C066A1CD694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094893D2-5656-4386-87E4-F9D84A5F9595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="24792" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="12480" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Git command" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>Command</t>
   </si>
@@ -79,6 +79,63 @@
   </si>
   <si>
     <t>Shows the current state of the working directory and the staging area</t>
+  </si>
+  <si>
+    <t>git commit -m</t>
+  </si>
+  <si>
+    <t>Save the staged changes with a commit message</t>
+  </si>
+  <si>
+    <t>git commit -m "message"</t>
+  </si>
+  <si>
+    <t>git log</t>
+  </si>
+  <si>
+    <t>Displays a log of all commits in the repository.</t>
+  </si>
+  <si>
+    <t>git log --all</t>
+  </si>
+  <si>
+    <t>git branch</t>
+  </si>
+  <si>
+    <t>List all branches in the repository</t>
+  </si>
+  <si>
+    <t>Creates a new branch</t>
+  </si>
+  <si>
+    <t>git branch (branch name)</t>
+  </si>
+  <si>
+    <t>git checkout -b</t>
+  </si>
+  <si>
+    <t>Creates and switches to a new branch</t>
+  </si>
+  <si>
+    <t>git checkout -b (branch name)</t>
+  </si>
+  <si>
+    <t>git merge</t>
+  </si>
+  <si>
+    <t>Merges another branch into the current branch</t>
+  </si>
+  <si>
+    <t>git merge (branch name)</t>
+  </si>
+  <si>
+    <t>git pull origin</t>
+  </si>
+  <si>
+    <t>Fetches and merges the latest changes from a remote repository</t>
+  </si>
+  <si>
+    <t>git pull origin (banch)</t>
   </si>
 </sst>
 </file>
@@ -406,10 +463,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B2:D8"/>
+  <dimension ref="B2:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -496,6 +553,83 @@
         <v>16</v>
       </c>
     </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>